<commit_message>
Updated spreadsheet format and added new info
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -11,39 +11,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Отметка времени</t>
   </si>
   <si>
-    <t>Фамилия</t>
-  </si>
-  <si>
-    <t>Имя</t>
-  </si>
-  <si>
-    <t>Курс</t>
-  </si>
-  <si>
-    <t>Адрес электронной почты</t>
-  </si>
-  <si>
-    <t>Адрес проживания</t>
-  </si>
-  <si>
-    <t>Пожелания</t>
-  </si>
-  <si>
-    <t>Аккаунт в социальной сети</t>
-  </si>
-  <si>
-    <t>Индекс</t>
+    <t>Фамилия (Surname)</t>
+  </si>
+  <si>
+    <t>Имя (Name)</t>
+  </si>
+  <si>
+    <t>Курс (Year)</t>
+  </si>
+  <si>
+    <t>Адрес электронной почты (Email)</t>
+  </si>
+  <si>
+    <t>Адрес проживания (Address)</t>
+  </si>
+  <si>
+    <t>Пожелания (Wishes)</t>
+  </si>
+  <si>
+    <t>Аккаунт в социальной сети (vk ID)</t>
+  </si>
+  <si>
+    <t>Индекс (Index)</t>
+  </si>
+  <si>
+    <t>Номер телефона (Phone number)</t>
   </si>
   <si>
     <t>Терова</t>
   </si>
   <si>
-    <t>Лера</t>
+    <t>Валерия</t>
   </si>
   <si>
     <t>terovaleriya@gmail.com</t>
@@ -52,16 +55,19 @@
     <t>Дудко 24</t>
   </si>
   <si>
-    <t>Винца</t>
-  </si>
-  <si>
-    <t>Караваева</t>
-  </si>
-  <si>
-    <t>Марина</t>
-  </si>
-  <si>
-    <t>2 магистратуры</t>
+    <t>Спать</t>
+  </si>
+  <si>
+    <t>+7-921-873-6059</t>
+  </si>
+  <si>
+    <t>Платонов</t>
+  </si>
+  <si>
+    <t>Платон</t>
+  </si>
+  <si>
+    <t>2 магистратуры (master)</t>
   </si>
   <si>
     <t>terova.valeriya2014@gmail.com</t>
@@ -70,10 +76,25 @@
     <t>Седова 24</t>
   </si>
   <si>
-    <t>Молока</t>
+    <t>Есть</t>
   </si>
   <si>
     <t>https://vk.com/terovaleriya</t>
+  </si>
+  <si>
+    <t>Препод</t>
+  </si>
+  <si>
+    <t>Степан</t>
+  </si>
+  <si>
+    <t>terovaleriya@ya.ru</t>
+  </si>
+  <si>
+    <t>14 линия</t>
+  </si>
+  <si>
+    <t>Умных студентов</t>
   </si>
 </sst>
 </file>
@@ -83,7 +104,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -93,6 +114,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <u/>
       <color rgb="FF0000FF"/>
@@ -112,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -120,10 +142,13 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -345,7 +370,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="15" width="21.57"/>
+    <col customWidth="1" min="1" max="16" width="21.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -376,60 +401,89 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3">
-        <v>44170.070424351856</v>
+      <c r="A2" s="4">
+        <v>44170.6170574537</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2">
         <v>2.0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I2" s="2">
-        <v>192148.0</v>
+        <v>45678.0</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3">
-        <v>44170.07107196759</v>
+      <c r="A3" s="4">
+        <v>44170.61825546296</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="I3" s="2">
-        <v>192437.0</v>
+        <v>456789.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4">
+        <v>44170.61911962963</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="2">
+        <v>3456765.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>